<commit_message>
added logic design for Material Bibliografico, including test data
</commit_message>
<xml_diff>
--- a/Diseños Lógicos.xlsx
+++ b/Diseños Lógicos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvict\OneDrive\Escritorio\VHCF\1-2024\Bases de datos I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvict\OneDrive\Escritorio\VHCF\Repositories\databases-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259CD9FF-411D-4EB0-B7F9-F28F97C2D247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD43B9A-94B7-4CA5-9976-FE41769C3B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="761" firstSheet="3" activeTab="10" xr2:uid="{A461B04F-0D6A-4D88-8CAA-5B9E37AF4F93}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="761" firstSheet="9" activeTab="11" xr2:uid="{A461B04F-0D6A-4D88-8CAA-5B9E37AF4F93}"/>
   </bookViews>
   <sheets>
     <sheet name="PELICULA" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="MAESTRODEOFERTA" sheetId="9" r:id="rId9"/>
     <sheet name="VEHICULO" sheetId="10" r:id="rId10"/>
     <sheet name="DISMAC" sheetId="11" r:id="rId11"/>
+    <sheet name="BIBLIOTECA" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="324">
   <si>
     <t>PELICULA</t>
   </si>
@@ -802,6 +803,222 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>MATERIAL_BIBLIO</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>FechaPublicacion</t>
+  </si>
+  <si>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>NroPaginas</t>
+  </si>
+  <si>
+    <t>Cien años de soledad</t>
+  </si>
+  <si>
+    <t>El Quijote</t>
+  </si>
+  <si>
+    <t>Clean Code</t>
+  </si>
+  <si>
+    <t>A Brief History of Time</t>
+  </si>
+  <si>
+    <t>Gabriel García Márquez</t>
+  </si>
+  <si>
+    <t>Miguel de Cervantes</t>
+  </si>
+  <si>
+    <t>Robert C. Martin</t>
+  </si>
+  <si>
+    <t>Stephen Hawking</t>
+  </si>
+  <si>
+    <t>1605-01-16</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>Inglés</t>
+  </si>
+  <si>
+    <t>LIBROS</t>
+  </si>
+  <si>
+    <t>EDITORIAL</t>
+  </si>
+  <si>
+    <t>Editorial Sudamericana</t>
+  </si>
+  <si>
+    <t>Editorial Planeta</t>
+  </si>
+  <si>
+    <t>Pearson</t>
+  </si>
+  <si>
+    <t>Bantam Books</t>
+  </si>
+  <si>
+    <t>Calle 123, Buenos Aires</t>
+  </si>
+  <si>
+    <t>Gran Vía 12, Madrid</t>
+  </si>
+  <si>
+    <t>221B Baker Street, London</t>
+  </si>
+  <si>
+    <t>375 Hudson Street, New York</t>
+  </si>
+  <si>
+    <t>TESIS</t>
+  </si>
+  <si>
+    <t>Grado</t>
+  </si>
+  <si>
+    <t>Universidad</t>
+  </si>
+  <si>
+    <t>Tutor</t>
+  </si>
+  <si>
+    <t>Doctorado</t>
+  </si>
+  <si>
+    <t>Licenciatura</t>
+  </si>
+  <si>
+    <t>Universidad Autónoma Gabriel René Moreno</t>
+  </si>
+  <si>
+    <t>Universidad Privada Boliviana</t>
+  </si>
+  <si>
+    <t>Dr. Joaquin Chumacero</t>
+  </si>
+  <si>
+    <t>Dr. Patricia Aguilera</t>
+  </si>
+  <si>
+    <t>Dr. Saturnino Mamani</t>
+  </si>
+  <si>
+    <t>Universidad Católica Boliviana</t>
+  </si>
+  <si>
+    <t>Universidad NUR</t>
+  </si>
+  <si>
+    <t>Dr. Josue Veizaga</t>
+  </si>
+  <si>
+    <t>PERIODICOS</t>
+  </si>
+  <si>
+    <t>Seccion</t>
+  </si>
+  <si>
+    <t>EditorialID</t>
+  </si>
+  <si>
+    <t>1967-05-30</t>
+  </si>
+  <si>
+    <t>2008-08-11</t>
+  </si>
+  <si>
+    <t>1988-04-01</t>
+  </si>
+  <si>
+    <t>The Pragmatic Programmer</t>
+  </si>
+  <si>
+    <t>Andrew Hunt</t>
+  </si>
+  <si>
+    <t>1999-10-20</t>
+  </si>
+  <si>
+    <t>Don Quijote de la Mancha</t>
+  </si>
+  <si>
+    <t>1615-11-01</t>
+  </si>
+  <si>
+    <t>To Kill a Mockingbird</t>
+  </si>
+  <si>
+    <t>Harper Lee</t>
+  </si>
+  <si>
+    <t>1960-07-11</t>
+  </si>
+  <si>
+    <t>Noticias</t>
+  </si>
+  <si>
+    <t>Maestría</t>
+  </si>
+  <si>
+    <t>Deportes</t>
+  </si>
+  <si>
+    <t>Economía</t>
+  </si>
+  <si>
+    <t>Cultura</t>
+  </si>
+  <si>
+    <t>NroEdicion</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>RevistaID</t>
+  </si>
+  <si>
+    <t>Investigación</t>
+  </si>
+  <si>
+    <t>Opinión</t>
+  </si>
+  <si>
+    <t>Crítica</t>
+  </si>
+  <si>
+    <t>Reportaje</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>789012</t>
+  </si>
+  <si>
+    <t>345678</t>
+  </si>
+  <si>
+    <t>901234</t>
+  </si>
+  <si>
+    <t>ARTICULOS</t>
+  </si>
+  <si>
+    <t>REVISTAS</t>
   </si>
 </sst>
 </file>
@@ -930,7 +1147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -989,46 +1206,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1057,6 +1268,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1655,34 +1868,34 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="47" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="47" t="s">
         <v>228</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="47" t="s">
         <v>229</v>
       </c>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="47" t="s">
         <v>241</v>
       </c>
     </row>
@@ -1775,7 +1988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2194223D-669E-4969-9A82-386E5AC46F87}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -1803,120 +2016,919 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="I3" s="49" t="s">
+      <c r="I3" s="45" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46">
+      <c r="A4" s="42">
         <v>111</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="42" t="s">
         <v>246</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="42">
         <v>7102030</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="42">
         <v>1000</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="42" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46">
+      <c r="A5" s="42">
         <v>222</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="42" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="42">
         <v>3561114</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="42">
         <v>700</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="42">
         <v>10</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="I5" s="42" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46">
+      <c r="A6" s="42">
         <v>333</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="42">
         <v>7210001</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="42">
         <v>15</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="42" t="s">
         <v>35</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D58926-4899-4BC9-9212-621AD7246594}">
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.6328125" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.90625" customWidth="1"/>
+    <col min="9" max="9" width="6.6328125" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="K3" s="53"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F4" s="2">
+        <v>471</v>
+      </c>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="2">
+        <v>863</v>
+      </c>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F6" s="2">
+        <v>464</v>
+      </c>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="53"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F7" s="2">
+        <v>256</v>
+      </c>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3</v>
+      </c>
+      <c r="K7" s="53"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F8" s="2">
+        <v>352</v>
+      </c>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4</v>
+      </c>
+      <c r="K8" s="53"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F9" s="2">
+        <v>940</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="2">
+        <v>6</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="53"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F10" s="2">
+        <v>281</v>
+      </c>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="2">
+        <v>7</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3</v>
+      </c>
+      <c r="K10" s="53"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+    </row>
+    <row r="12" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="2">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="2">
+        <v>3</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+    </row>
+    <row r="21" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
+        <v>23</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="2">
+        <v>2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>45</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="2">
+        <v>3</v>
+      </c>
+      <c r="J27" s="2">
+        <v>12</v>
+      </c>
+      <c r="K27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="2">
+        <v>4</v>
+      </c>
+      <c r="J28" s="2">
+        <v>30</v>
+      </c>
+      <c r="K28" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="K33" s="24" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="2">
+        <v>1</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="2">
+        <v>2</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="2">
+        <v>3</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="K36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="2">
+        <v>4</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="K37" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="52"/>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2845,7 +3857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71621443-0F11-446A-86BC-C88F46F8DB9C}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+    <sheetView topLeftCell="AE1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
@@ -4114,8 +5126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F885D0-7CC3-4D90-9E76-D1E1C60CD759}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4411,101 +5423,96 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="33"/>
-    <col min="2" max="2" width="32.81640625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="3" style="33" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="33"/>
-    <col min="5" max="5" width="9.81640625" style="33" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" style="33" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="33"/>
-    <col min="8" max="8" width="10.54296875" style="33" customWidth="1"/>
-    <col min="9" max="9" width="8" style="33" customWidth="1"/>
-    <col min="10" max="10" width="10.90625" style="33" customWidth="1"/>
-    <col min="11" max="12" width="9.81640625" style="33" customWidth="1"/>
-    <col min="13" max="13" width="4.08984375" style="33" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="33"/>
-    <col min="15" max="15" width="11.453125" style="33" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="33"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="3" max="3" width="3" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="10.90625" customWidth="1"/>
+    <col min="11" max="12" width="9.81640625" customWidth="1"/>
+    <col min="13" max="13" width="4.08984375" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="31" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="N1" s="30" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="N1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="30"/>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="N2" s="30" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="N2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="30"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="52" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="32"/>
+      <c r="I3" s="31"/>
       <c r="J3" s="17" t="s">
         <v>7</v>
       </c>
@@ -4515,448 +5522,448 @@
       <c r="L3" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="M3" s="32"/>
-      <c r="N3" s="52" t="s">
+      <c r="M3" s="31"/>
+      <c r="N3" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="O3" s="52" t="s">
+      <c r="O3" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="P3" s="53" t="s">
+      <c r="P3" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="Q3" s="53" t="s">
+      <c r="Q3" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="R3" s="53" t="s">
+      <c r="R3" s="49" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="34">
+      <c r="A4" s="32">
         <v>111</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="34">
+      <c r="C4" s="31"/>
+      <c r="D4" s="32">
         <v>100</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="32">
         <v>111</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="33">
         <v>1</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="35">
+      <c r="I4" s="31"/>
+      <c r="J4" s="7">
         <v>1</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4" s="7">
         <v>1</v>
       </c>
-      <c r="L4" s="35">
+      <c r="L4" s="7">
         <v>2024</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="34">
+      <c r="M4" s="31"/>
+      <c r="N4" s="32">
         <v>100</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="32">
         <v>1</v>
       </c>
-      <c r="P4" s="36" t="s">
+      <c r="P4" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Q4" s="37">
+      <c r="Q4" s="34">
         <v>0.38541666666666669</v>
       </c>
-      <c r="R4" s="37">
+      <c r="R4" s="34">
         <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="34">
+      <c r="A5" s="32">
         <v>222</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="34">
+      <c r="C5" s="31"/>
+      <c r="D5" s="32">
         <v>101</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="32">
         <v>222</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="33">
         <v>1</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="35">
+      <c r="I5" s="31"/>
+      <c r="J5" s="7">
         <v>2</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="7">
         <v>2</v>
       </c>
-      <c r="L5" s="35">
+      <c r="L5" s="7">
         <v>2024</v>
       </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="34">
+      <c r="M5" s="31"/>
+      <c r="N5" s="32">
         <v>100</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="32">
         <v>2</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="Q5" s="37">
+      <c r="Q5" s="34">
         <v>0.38541666666666669</v>
       </c>
-      <c r="R5" s="37">
+      <c r="R5" s="34">
         <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="34">
+      <c r="A6" s="32">
         <v>333</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="34">
+      <c r="C6" s="31"/>
+      <c r="D6" s="32">
         <v>102</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="32">
         <v>333</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="33">
         <v>1</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="34">
+      <c r="I6" s="31"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32">
         <v>101</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6" s="32">
         <v>1</v>
       </c>
-      <c r="P6" s="36" t="s">
+      <c r="P6" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="Q6" s="37">
+      <c r="Q6" s="34">
         <v>0.57291666666666663</v>
       </c>
-      <c r="R6" s="37">
+      <c r="R6" s="34">
         <v>0.63541666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="34">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32">
         <v>103</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="32">
         <v>111</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="33">
         <v>1</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="34">
+      <c r="I7" s="31"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32">
         <v>101</v>
       </c>
-      <c r="O7" s="34">
+      <c r="O7" s="32">
         <v>2</v>
       </c>
-      <c r="P7" s="36" t="s">
+      <c r="P7" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="Q7" s="37">
+      <c r="Q7" s="34">
         <v>0.57291666666666663</v>
       </c>
-      <c r="R7" s="37">
+      <c r="R7" s="34">
         <v>0.63541666666666663</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="34">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32">
         <v>104</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="32">
         <v>111</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="33">
         <v>1</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="34">
+      <c r="I8" s="31"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="32">
         <v>101</v>
       </c>
-      <c r="O8" s="34">
+      <c r="O8" s="32">
         <v>3</v>
       </c>
-      <c r="P8" s="36" t="s">
+      <c r="P8" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="Q8" s="37">
+      <c r="Q8" s="34">
         <v>0.57291666666666663</v>
       </c>
-      <c r="R8" s="37">
+      <c r="R8" s="34">
         <v>0.63541666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="34">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32">
         <v>105</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="32">
         <v>111</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="32">
         <v>2</v>
       </c>
-      <c r="I9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="34">
+      <c r="I9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="32">
         <v>102</v>
       </c>
-      <c r="O9" s="34">
+      <c r="O9" s="32">
         <v>1</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="Q9" s="37">
+      <c r="Q9" s="34">
         <v>0.29166666666666669</v>
       </c>
-      <c r="R9" s="37">
+      <c r="R9" s="34">
         <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="34">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="32">
         <v>102</v>
       </c>
-      <c r="O10" s="34">
+      <c r="O10" s="32">
         <v>2</v>
       </c>
-      <c r="P10" s="36" t="s">
+      <c r="P10" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="Q10" s="37">
+      <c r="Q10" s="34">
         <v>0.29166666666666669</v>
       </c>
-      <c r="R10" s="37">
+      <c r="R10" s="34">
         <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="34">
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="32">
         <v>102</v>
       </c>
-      <c r="O11" s="34">
+      <c r="O11" s="32">
         <v>3</v>
       </c>
-      <c r="P11" s="36" t="s">
+      <c r="P11" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="34">
         <v>0.29166666666666669</v>
       </c>
-      <c r="R11" s="37">
+      <c r="R11" s="34">
         <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="35">
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="7">
         <v>103</v>
       </c>
-      <c r="O12" s="34">
+      <c r="O12" s="32">
         <v>1</v>
       </c>
-      <c r="P12" s="36" t="s">
+      <c r="P12" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q12" s="35">
         <v>0.35416666666666669</v>
       </c>
-      <c r="R12" s="38">
+      <c r="R12" s="35">
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="32"/>
-      <c r="E13" s="39" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="31"/>
+      <c r="E13" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="32"/>
-      <c r="I13" s="31" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="31"/>
+      <c r="I13" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="35">
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="7">
         <v>103</v>
       </c>
-      <c r="O13" s="34">
+      <c r="O13" s="32">
         <v>2</v>
       </c>
-      <c r="P13" s="36" t="s">
+      <c r="P13" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="Q13" s="38">
+      <c r="Q13" s="35">
         <v>0.35416666666666669</v>
       </c>
-      <c r="R13" s="38">
+      <c r="R13" s="35">
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="32"/>
-      <c r="E14" s="39" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="31"/>
+      <c r="E14" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="32"/>
-      <c r="I14" s="31" t="s">
+      <c r="F14" s="36"/>
+      <c r="G14" s="31"/>
+      <c r="I14" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="35">
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="7">
         <v>103</v>
       </c>
-      <c r="O14" s="34">
+      <c r="O14" s="32">
         <v>3</v>
       </c>
-      <c r="P14" s="36" t="s">
+      <c r="P14" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="Q14" s="38">
+      <c r="Q14" s="35">
         <v>0.35416666666666669</v>
       </c>
-      <c r="R14" s="38">
+      <c r="R14" s="35">
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="E15" s="55" t="s">
+      <c r="C15" s="31"/>
+      <c r="E15" s="51" t="s">
         <v>80</v>
       </c>
       <c r="F15" s="18" t="s">
@@ -4977,367 +5984,367 @@
       <c r="L15" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="M15" s="32"/>
-      <c r="N15" s="35">
+      <c r="M15" s="31"/>
+      <c r="N15" s="7">
         <v>104</v>
       </c>
-      <c r="O15" s="34">
+      <c r="O15" s="32">
         <v>1</v>
       </c>
-      <c r="P15" s="35" t="s">
+      <c r="P15" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="Q15" s="38">
+      <c r="Q15" s="35">
         <v>0.29166666666666669</v>
       </c>
-      <c r="R15" s="38">
+      <c r="R15" s="35">
         <v>0.38541666666666669</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="E16" s="40">
+      <c r="C16" s="31"/>
+      <c r="E16" s="9">
         <v>202401</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G16" s="7">
         <v>7102030</v>
       </c>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42">
+      <c r="H16" s="37"/>
+      <c r="I16" s="38">
         <v>1</v>
       </c>
-      <c r="J16" s="43">
+      <c r="J16" s="39">
         <v>45361</v>
       </c>
-      <c r="K16" s="44">
+      <c r="K16" s="40">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L16" s="35">
+      <c r="L16" s="7">
         <v>202401</v>
       </c>
-      <c r="M16" s="32"/>
-      <c r="N16" s="35">
+      <c r="M16" s="31"/>
+      <c r="N16" s="7">
         <v>104</v>
       </c>
-      <c r="O16" s="34">
+      <c r="O16" s="32">
         <v>2</v>
       </c>
-      <c r="P16" s="35" t="s">
+      <c r="P16" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="Q16" s="38">
+      <c r="Q16" s="35">
         <v>0.29166666666666669</v>
       </c>
-      <c r="R16" s="38">
+      <c r="R16" s="35">
         <v>0.38541666666666669</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="E17" s="40">
+      <c r="C17" s="31"/>
+      <c r="E17" s="9">
         <v>202402</v>
       </c>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="7">
         <v>3568999</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="42">
+      <c r="H17" s="37"/>
+      <c r="I17" s="38">
         <v>2</v>
       </c>
-      <c r="J17" s="43">
+      <c r="J17" s="39">
         <v>45363</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="40">
         <v>0.375</v>
       </c>
-      <c r="L17" s="35">
+      <c r="L17" s="7">
         <v>202402</v>
       </c>
-      <c r="M17" s="32"/>
-      <c r="N17" s="35">
+      <c r="M17" s="31"/>
+      <c r="N17" s="7">
         <v>105</v>
       </c>
-      <c r="O17" s="35">
+      <c r="O17" s="7">
         <v>1</v>
       </c>
-      <c r="P17" s="35" t="s">
+      <c r="P17" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="Q17" s="37">
+      <c r="Q17" s="34">
         <v>0.38541666666666669</v>
       </c>
-      <c r="R17" s="37">
+      <c r="R17" s="34">
         <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="32"/>
-      <c r="E18" s="40">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="31"/>
+      <c r="E18" s="9">
         <v>202403</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="G18" s="35">
+      <c r="G18" s="7">
         <v>7828288</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42">
+      <c r="H18" s="37"/>
+      <c r="I18" s="38">
         <v>3</v>
       </c>
-      <c r="J18" s="43">
+      <c r="J18" s="39">
         <v>45363</v>
       </c>
-      <c r="K18" s="44">
+      <c r="K18" s="40">
         <v>0.38541666666666669</v>
       </c>
-      <c r="L18" s="35">
+      <c r="L18" s="7">
         <v>202403</v>
       </c>
-      <c r="M18" s="32"/>
-      <c r="N18" s="35">
+      <c r="M18" s="31"/>
+      <c r="N18" s="7">
         <v>105</v>
       </c>
-      <c r="O18" s="35">
+      <c r="O18" s="7">
         <v>2</v>
       </c>
-      <c r="P18" s="35" t="s">
+      <c r="P18" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="Q18" s="37">
+      <c r="Q18" s="34">
         <v>0.38541666666666669</v>
       </c>
-      <c r="R18" s="37">
+      <c r="R18" s="34">
         <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="32"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="31"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="32"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="31"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="32"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="31"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="32"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="31"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="32"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="32"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="E26" s="30" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="E26" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="32"/>
+      <c r="F26" s="1"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E28" s="50" t="s">
+      <c r="E28" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F28" s="50" t="s">
+      <c r="F28" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E29" s="40">
+      <c r="E29" s="9">
         <v>1</v>
       </c>
-      <c r="F29" s="40">
+      <c r="F29" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E30" s="40">
+      <c r="E30" s="9">
         <v>1</v>
       </c>
-      <c r="F30" s="40">
+      <c r="F30" s="9">
         <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E31" s="40">
+      <c r="E31" s="9">
         <v>2</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="9">
         <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E32" s="40">
+      <c r="E32" s="9">
         <v>3</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="9">
         <v>101</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E33" s="40">
+      <c r="E33" s="9">
         <v>3</v>
       </c>
-      <c r="F33" s="40">
+      <c r="F33" s="9">
         <v>104</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enhanced logic design deleting unnecessary and non-relationed items
</commit_message>
<xml_diff>
--- a/Diseños Lógicos.xlsx
+++ b/Diseños Lógicos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvict\OneDrive\Escritorio\VHCF\Repositories\databases-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD43B9A-94B7-4CA5-9976-FE41769C3B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A748086-139C-410F-9107-DE861AB1998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="761" firstSheet="9" activeTab="11" xr2:uid="{A461B04F-0D6A-4D88-8CAA-5B9E37AF4F93}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="330">
   <si>
     <t>PELICULA</t>
   </si>
@@ -829,9 +829,6 @@
     <t>Clean Code</t>
   </si>
   <si>
-    <t>A Brief History of Time</t>
-  </si>
-  <si>
     <t>Gabriel García Márquez</t>
   </si>
   <si>
@@ -841,9 +838,6 @@
     <t>Robert C. Martin</t>
   </si>
   <si>
-    <t>Stephen Hawking</t>
-  </si>
-  <si>
     <t>1605-01-16</t>
   </si>
   <si>
@@ -904,24 +898,12 @@
     <t>Universidad Autónoma Gabriel René Moreno</t>
   </si>
   <si>
-    <t>Universidad Privada Boliviana</t>
-  </si>
-  <si>
     <t>Dr. Joaquin Chumacero</t>
   </si>
   <si>
-    <t>Dr. Patricia Aguilera</t>
-  </si>
-  <si>
-    <t>Dr. Saturnino Mamani</t>
-  </si>
-  <si>
     <t>Universidad Católica Boliviana</t>
   </si>
   <si>
-    <t>Universidad NUR</t>
-  </si>
-  <si>
     <t>Dr. Josue Veizaga</t>
   </si>
   <si>
@@ -940,9 +922,6 @@
     <t>2008-08-11</t>
   </si>
   <si>
-    <t>1988-04-01</t>
-  </si>
-  <si>
     <t>The Pragmatic Programmer</t>
   </si>
   <si>
@@ -952,36 +931,12 @@
     <t>1999-10-20</t>
   </si>
   <si>
-    <t>Don Quijote de la Mancha</t>
-  </si>
-  <si>
-    <t>1615-11-01</t>
-  </si>
-  <si>
-    <t>To Kill a Mockingbird</t>
-  </si>
-  <si>
-    <t>Harper Lee</t>
-  </si>
-  <si>
-    <t>1960-07-11</t>
-  </si>
-  <si>
     <t>Noticias</t>
   </si>
   <si>
-    <t>Maestría</t>
-  </si>
-  <si>
     <t>Deportes</t>
   </si>
   <si>
-    <t>Economía</t>
-  </si>
-  <si>
-    <t>Cultura</t>
-  </si>
-  <si>
     <t>NroEdicion</t>
   </si>
   <si>
@@ -997,12 +952,6 @@
     <t>Opinión</t>
   </si>
   <si>
-    <t>Crítica</t>
-  </si>
-  <si>
-    <t>Reportaje</t>
-  </si>
-  <si>
     <t>123456</t>
   </si>
   <si>
@@ -1019,6 +968,75 @@
   </si>
   <si>
     <t>REVISTAS</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Estudio sobre la economía</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>Investigación en IA</t>
+  </si>
+  <si>
+    <t>2019-06-15</t>
+  </si>
+  <si>
+    <t>Periodico Noticias</t>
+  </si>
+  <si>
+    <t>2022-12-01</t>
+  </si>
+  <si>
+    <t>Periodico Deportes</t>
+  </si>
+  <si>
+    <t>2022-12-02</t>
+  </si>
+  <si>
+    <t>Revista de Ciencia</t>
+  </si>
+  <si>
+    <t>2022-11-01</t>
+  </si>
+  <si>
+    <t>Revista de Tecnología</t>
+  </si>
+  <si>
+    <t>2022-10-01</t>
+  </si>
+  <si>
+    <t>Artículo de Investigación</t>
+  </si>
+  <si>
+    <t>2021-08-15</t>
+  </si>
+  <si>
+    <t>Artículo de Opinión</t>
+  </si>
+  <si>
+    <t>Michael Brown</t>
+  </si>
+  <si>
+    <t>2021-09-10</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Gabriel Salinas</t>
+  </si>
+  <si>
+    <t>Ariel Mendez</t>
   </si>
 </sst>
 </file>
@@ -1268,8 +1286,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2138,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D58926-4899-4BC9-9212-621AD7246594}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2152,13 +2170,14 @@
     <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.90625" customWidth="1"/>
-    <col min="9" max="9" width="6.6328125" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.90625" customWidth="1"/>
+    <col min="10" max="10" width="6.6328125" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>252</v>
       </c>
@@ -2169,12 +2188,13 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2185,750 +2205,643 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="23" t="s">
+      <c r="G3" s="53" t="s">
+        <v>297</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="K3" s="53"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="K3" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="C4" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" s="9">
         <v>471</v>
       </c>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="2">
-        <v>1</v>
+      <c r="G4" s="8" t="s">
+        <v>307</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" s="9">
+        <v>863</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F5" s="2">
-        <v>863</v>
-      </c>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="2">
+      <c r="F6" s="9">
+        <v>464</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>293</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="9">
+        <v>352</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2">
         <v>2</v>
       </c>
-      <c r="J5" s="2">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" s="9">
+        <v>150</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F9" s="9">
+        <v>200</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F10" s="9">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F11" s="9">
+        <v>28</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F12" s="9">
+        <v>50</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F13" s="9">
+        <v>48</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="J13" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="53"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="K13" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F14" s="9">
+        <v>20</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F15" s="9">
+        <v>15</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="L21" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="2">
+        <v>8</v>
+      </c>
+      <c r="K22" s="2">
+        <v>23</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J23" s="2">
+        <v>9</v>
+      </c>
+      <c r="K23" s="2">
+        <v>45</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F6" s="2">
-        <v>464</v>
-      </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="2">
-        <v>3</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="B30" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="L30" s="20" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="2">
+        <v>11</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J32" s="2">
+        <v>12</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="L32" s="2">
         <v>2</v>
       </c>
-      <c r="K6" s="53"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F7" s="2">
-        <v>256</v>
-      </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="2">
-        <v>4</v>
-      </c>
-      <c r="J7" s="2">
-        <v>3</v>
-      </c>
-      <c r="K7" s="53"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F8" s="2">
-        <v>352</v>
-      </c>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="2">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2">
-        <v>4</v>
-      </c>
-      <c r="K8" s="53"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F9" s="2">
-        <v>940</v>
-      </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="2">
-        <v>6</v>
-      </c>
-      <c r="J9" s="2">
-        <v>2</v>
-      </c>
-      <c r="K9" s="53"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" s="2">
-        <v>281</v>
-      </c>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="2">
-        <v>7</v>
-      </c>
-      <c r="J10" s="2">
-        <v>3</v>
-      </c>
-      <c r="K10" s="53"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-    </row>
-    <row r="12" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="2">
-        <v>2</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="K17" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>3</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="2">
-        <v>3</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>4</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="2">
-        <v>4</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="K19" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-    </row>
-    <row r="21" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="2">
-        <v>1</v>
-      </c>
-      <c r="J25" s="2">
-        <v>23</v>
-      </c>
-      <c r="K25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="2">
-        <v>2</v>
-      </c>
-      <c r="J26" s="2">
-        <v>45</v>
-      </c>
-      <c r="K26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
-        <v>3</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="2">
-        <v>3</v>
-      </c>
-      <c r="J27" s="2">
-        <v>12</v>
-      </c>
-      <c r="K27" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
-        <v>4</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="2">
-        <v>4</v>
-      </c>
-      <c r="J28" s="2">
-        <v>30</v>
-      </c>
-      <c r="K28" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="K33" s="24" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="2">
-        <v>1</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="K34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="2">
-        <v>2</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="K35" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="2">
-        <v>3</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="K36" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="2">
-        <v>4</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="K37" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-    </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-    </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
+    </row>
+    <row r="33" spans="10:12" x14ac:dyDescent="0.35">
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="10:12" x14ac:dyDescent="0.35">
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Library design by Veizaga
</commit_message>
<xml_diff>
--- a/Diseños Lógicos.xlsx
+++ b/Diseños Lógicos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvict\OneDrive\Escritorio\VHCF\Repositories\databases-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A748086-139C-410F-9107-DE861AB1998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E601BC-B9F3-4965-9B0B-FDAA6857B0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="761" firstSheet="9" activeTab="11" xr2:uid="{A461B04F-0D6A-4D88-8CAA-5B9E37AF4F93}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="MAESTRODEOFERTA" sheetId="9" r:id="rId9"/>
     <sheet name="VEHICULO" sheetId="10" r:id="rId10"/>
     <sheet name="DISMAC" sheetId="11" r:id="rId11"/>
-    <sheet name="BIBLIOTECA" sheetId="12" r:id="rId12"/>
+    <sheet name="BIBLIOTECA" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="269">
   <si>
     <t>PELICULA</t>
   </si>
@@ -805,238 +805,55 @@
     <t>null</t>
   </si>
   <si>
-    <t>MATERIAL_BIBLIO</t>
-  </si>
-  <si>
-    <t>Autor</t>
-  </si>
-  <si>
-    <t>FechaPublicacion</t>
-  </si>
-  <si>
-    <t>Idioma</t>
-  </si>
-  <si>
-    <t>NroPaginas</t>
-  </si>
-  <si>
-    <t>Cien años de soledad</t>
-  </si>
-  <si>
-    <t>El Quijote</t>
-  </si>
-  <si>
-    <t>Clean Code</t>
-  </si>
-  <si>
-    <t>Gabriel García Márquez</t>
-  </si>
-  <si>
-    <t>Miguel de Cervantes</t>
-  </si>
-  <si>
-    <t>Robert C. Martin</t>
-  </si>
-  <si>
-    <t>1605-01-16</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
-    <t>Inglés</t>
-  </si>
-  <si>
-    <t>LIBROS</t>
-  </si>
-  <si>
-    <t>EDITORIAL</t>
-  </si>
-  <si>
-    <t>Editorial Sudamericana</t>
-  </si>
-  <si>
-    <t>Editorial Planeta</t>
-  </si>
-  <si>
-    <t>Pearson</t>
-  </si>
-  <si>
-    <t>Bantam Books</t>
-  </si>
-  <si>
-    <t>Calle 123, Buenos Aires</t>
-  </si>
-  <si>
-    <t>Gran Vía 12, Madrid</t>
-  </si>
-  <si>
-    <t>221B Baker Street, London</t>
-  </si>
-  <si>
-    <t>375 Hudson Street, New York</t>
-  </si>
-  <si>
     <t>TESIS</t>
   </si>
   <si>
-    <t>Grado</t>
-  </si>
-  <si>
-    <t>Universidad</t>
-  </si>
-  <si>
     <t>Tutor</t>
   </si>
   <si>
-    <t>Doctorado</t>
-  </si>
-  <si>
-    <t>Licenciatura</t>
-  </si>
-  <si>
-    <t>Universidad Autónoma Gabriel René Moreno</t>
-  </si>
-  <si>
-    <t>Dr. Joaquin Chumacero</t>
-  </si>
-  <si>
-    <t>Universidad Católica Boliviana</t>
-  </si>
-  <si>
-    <t>Dr. Josue Veizaga</t>
-  </si>
-  <si>
-    <t>PERIODICOS</t>
-  </si>
-  <si>
-    <t>Seccion</t>
-  </si>
-  <si>
-    <t>EditorialID</t>
-  </si>
-  <si>
-    <t>1967-05-30</t>
-  </si>
-  <si>
-    <t>2008-08-11</t>
-  </si>
-  <si>
-    <t>The Pragmatic Programmer</t>
-  </si>
-  <si>
-    <t>Andrew Hunt</t>
-  </si>
-  <si>
-    <t>1999-10-20</t>
-  </si>
-  <si>
-    <t>Noticias</t>
-  </si>
-  <si>
-    <t>Deportes</t>
-  </si>
-  <si>
-    <t>NroEdicion</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
-    <t>RevistaID</t>
-  </si>
-  <si>
-    <t>Investigación</t>
-  </si>
-  <si>
-    <t>Opinión</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>789012</t>
-  </si>
-  <si>
-    <t>345678</t>
-  </si>
-  <si>
-    <t>901234</t>
-  </si>
-  <si>
-    <t>ARTICULOS</t>
-  </si>
-  <si>
-    <t>REVISTAS</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Estudio sobre la economía</t>
-  </si>
-  <si>
-    <t>2020-01-01</t>
-  </si>
-  <si>
-    <t>Investigación en IA</t>
-  </si>
-  <si>
-    <t>2019-06-15</t>
-  </si>
-  <si>
-    <t>Periodico Noticias</t>
-  </si>
-  <si>
-    <t>2022-12-01</t>
-  </si>
-  <si>
-    <t>Periodico Deportes</t>
-  </si>
-  <si>
-    <t>2022-12-02</t>
-  </si>
-  <si>
-    <t>Revista de Ciencia</t>
-  </si>
-  <si>
-    <t>2022-11-01</t>
-  </si>
-  <si>
-    <t>Revista de Tecnología</t>
-  </si>
-  <si>
-    <t>2022-10-01</t>
-  </si>
-  <si>
-    <t>Artículo de Investigación</t>
-  </si>
-  <si>
-    <t>2021-08-15</t>
-  </si>
-  <si>
-    <t>Artículo de Opinión</t>
-  </si>
-  <si>
-    <t>Michael Brown</t>
-  </si>
-  <si>
-    <t>2021-09-10</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Gabriel Salinas</t>
-  </si>
-  <si>
-    <t>Ariel Mendez</t>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>MATERIALBIBLIOGRAFICO</t>
+  </si>
+  <si>
+    <t>NroPag</t>
+  </si>
+  <si>
+    <t>FICHAPRESTAMO</t>
+  </si>
+  <si>
+    <t>Editorial</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>FechaDev</t>
+  </si>
+  <si>
+    <t>LIBRO</t>
+  </si>
+  <si>
+    <t>AñoPub</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Edicion</t>
+  </si>
+  <si>
+    <t>REVISTA</t>
+  </si>
+  <si>
+    <t>CIPersona</t>
+  </si>
+  <si>
+    <t>CodigoMB</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -1286,8 +1103,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1828,7 +1643,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2007,7 +1822,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2155,693 +1970,354 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D58926-4899-4BC9-9212-621AD7246594}">
-  <dimension ref="A1:L34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AD5D36-8052-4054-8001-6CA6365D1075}">
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.90625" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" customWidth="1"/>
+    <col min="13" max="13" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>252</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>266</v>
-      </c>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="I3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>297</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="L3" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="F4" s="9">
-        <v>471</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="N3" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="F5" s="9">
-        <v>863</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="9">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="P3" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F6" s="9">
-        <v>464</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="J6" s="2">
-        <v>3</v>
-      </c>
-      <c r="K6" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="9">
-        <v>4</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>293</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F7" s="9">
-        <v>352</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="J7" s="2">
-        <v>4</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <v>5</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F8" s="9">
-        <v>150</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F9" s="9">
-        <v>200</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>7</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="F10" s="9">
-        <v>30</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>286</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="9">
-        <v>8</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="F11" s="9">
-        <v>28</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>227</v>
-      </c>
+      <c r="L10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F12" s="9">
-        <v>50</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="L12" s="20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
-        <v>10</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="F13" s="9">
-        <v>48</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="L13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <v>11</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="E12" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="F14" s="9">
-        <v>20</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="J14" s="2">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="G12" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
       <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
-        <v>12</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F15" s="9">
-        <v>15</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
       <c r="L16" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="J19" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
-        <v>5</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="L21" s="20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="2">
-        <v>8</v>
-      </c>
-      <c r="K22" s="2">
-        <v>23</v>
-      </c>
-      <c r="L22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J23" s="2">
-        <v>9</v>
-      </c>
-      <c r="K23" s="2">
-        <v>45</v>
-      </c>
-      <c r="L23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
-        <v>1</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="J28" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
-        <v>2</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
-        <v>3</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="L30" s="20" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
-        <v>4</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="2">
-        <v>11</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J32" s="2">
-        <v>12</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="L32" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="10:12" x14ac:dyDescent="0.35">
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="10:12" x14ac:dyDescent="0.35">
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>